<commit_message>
Import-Pupil besser nun mit xlsx
</commit_message>
<xml_diff>
--- a/Diklabu/PowerShell/schueler.xlsx
+++ b/Diklabu/PowerShell/schueler.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>GEBDAT</t>
   </si>
@@ -36,16 +36,19 @@
     <t>Jörg</t>
   </si>
   <si>
-    <t>Joerg</t>
-  </si>
-  <si>
-    <t>Frank</t>
-  </si>
-  <si>
     <t>KNAME</t>
   </si>
   <si>
+    <t>ID_LEHRER</t>
+  </si>
+  <si>
+    <t>ID_KATEGORIE</t>
+  </si>
+  <si>
     <t>FIAE17A</t>
+  </si>
+  <si>
+    <t>HK</t>
   </si>
 </sst>
 </file>
@@ -53,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -484,20 +487,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="3" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.265625" customWidth="1"/>
+    <col min="6" max="6" width="14.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -507,10 +511,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>24939</v>
       </c>
@@ -520,36 +530,20 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>24939</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>24940</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>

</xml_diff>